<commit_message>
feat: get more examples
</commit_message>
<xml_diff>
--- a/SFData/StackOverflow.xlsx
+++ b/SFData/StackOverflow.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t xml:space="preserve">question id</t>
   </si>
@@ -44,6 +44,43 @@
   </si>
   <si>
     <t xml:space="preserve">exception content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-05-01 21:20:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TensorFlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-  train_step.run(feed_dict={x: x1[0], y_: y1[0]})
++  train_step.run(feed_dict={x: np.expand_dims(x1[0], 0), y_: np.expand_dims(y1[0], 0)})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature Input Incompatible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature Data Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValueError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot feed value of shape (19,) for Tensor 'Placeholder:0', which has shape '(?, 19)'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-08-18 04:03:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+char_num_steps = [char_num_steps]*batch_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter Restriction Incompatible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OP Parameter Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequence_length must be a vector of length batch_size, but saw shape: ()</t>
   </si>
   <si>
     <t xml:space="preserve">2017-02-14 20:29:54</t>
@@ -60,9 +97,6 @@
   </si>
   <si>
     <t xml:space="preserve">Model Output Shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ValueError</t>
   </si>
   <si>
     <t xml:space="preserve">A target array with shape (100, 1) was passed for an output of shape (None, 4) while using as loss `mean_squared_error`. This loss expects targets to have the same shape as the output.</t>
@@ -189,10 +223,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.44"/>
@@ -232,7 +266,7 @@
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>42235611</v>
+        <v>36972087</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>8</v>
@@ -256,8 +290,58 @@
         <v>14</v>
       </c>
     </row>
-    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>39009808</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>42235611</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>